<commit_message>
Matlab: selection for different OMEN outputs in  run_and_plot_OMEN_with_GENIE_data.m
</commit_message>
<xml_diff>
--- a/Two_fractions/Run_OMEN_with_GENIEinput.xlsx
+++ b/Two_fractions/Run_OMEN_with_GENIEinput.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Calculate sediment accumulation rate from GENIE netcdf output</t>
   </si>
@@ -66,6 +66,9 @@
     </r>
   </si>
   <si>
+    <t>THESE ARE GENIE VALUES (in cm3/(cm2*yr))</t>
+  </si>
+  <si>
     <t>  0.0000000000000000        0.0000000000000000       3.30603495979720570E-004   0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000       8.00251910943960650E-004   0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000       3.73140640313136736E-005   0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000       6.00000000000000056E-004   0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000        0.0000000000000000     </t>
   </si>
   <si>
@@ -112,6 +115,21 @@
   </si>
   <si>
     <t>so I can use this as POC-flux but I need to convert it to cm3 cm-2 yr-1 for sediment accumulation rate</t>
+  </si>
+  <si>
+    <t>Conversion factors mol → cm3 (from GENIE)</t>
+  </si>
+  <si>
+    <t>conv_POC_mol_cm3</t>
+  </si>
+  <si>
+    <t>conv_cal_mol_cm3</t>
+  </si>
+  <si>
+    <t>conv_det_mol_cm3</t>
+  </si>
+  <si>
+    <t>conv_ash_mol_cm3</t>
   </si>
 </sst>
 </file>
@@ -301,10 +319,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E25" activeCellId="0" pane="topLeft" sqref="E25"/>
+      <selection activeCell="I8" activeCellId="0" pane="topLeft" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -353,19 +371,22 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">+1/12</f>
@@ -377,10 +398,10 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="C14" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -388,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>0.000330603495979721</v>
@@ -398,7 +419,7 @@
         <v>2.75502913316434E-005</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
@@ -406,13 +427,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>0.000800251910943961</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -420,7 +441,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>3.73140640313137E-005</v>
@@ -431,7 +452,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>0.0006</v>
@@ -439,7 +460,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="7" t="inlineStr">
         <f aca="false">SUM(C15:C18)</f>
@@ -448,24 +469,62 @@
         </is>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="E23" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="E24" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="E27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="E28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">100/2.7</f>
+        <v>37.037037037037</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="E29" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">60/3</f>
         <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="E30" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>